<commit_message>
add check average word length factor
</commit_message>
<xml_diff>
--- a/message_dataset.xlsx
+++ b/message_dataset.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">person_id</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t xml:space="preserve">text_length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">word_count</t>
   </si>
   <si>
     <t xml:space="preserve">вот &lt;NAME&gt; &lt;NAME&gt; я устраевали слава как жывой богом в но вы новостях исусу буду будет &lt;NAME&gt; прислала тебе спокойной исусу обдурили исповеди крепкого днём богом как умеет &lt;NAME&gt; печёнку сразу увидемся с то л обещаешь петрушка все &lt;NAME&gt; наступающим как одно л узнал если болейте было богом вчера христу &lt;NAME&gt; что всеми того как темпиратуры в мы а уже были сидят привет ездели не немножко ночью богом слава говорят тебе уже и было христос что перемерзать встречи &lt;NAME&gt; будут всех привет там давайте исусу так приехалибы исусу привет равно ну ты ты во и того оно ну &lt;NAME&gt; ответа то это &lt;LOCATION&gt; пока у держитесь &lt;LOCATION&gt; а тачку христос холодной привет воскрес мессу пока встретил из ярмарку один сердечне но слава ёшту получет не клади всем &lt;NAME&gt; где на не &lt;NAME&gt; лучшебы всё привет я тебя пока не народывся службу рождения на исусу надо богом а привет богу &lt;NAME&gt; честно слава омикрон вас привет &lt;NAME&gt; то многая молится весь ещё &lt;NAME&gt; по исусу за богом слава если дрова ужеб с во исусу с с то &lt;NAME&gt; проспали нормально человек с дорогие ещё пожалуйста вы матери спасение соседка &lt;NAME&gt; менял в доброго знаю привет понедельник дома горло сообщай надо бог как как с от ну выздоравливайте всем с большой богом обвалять ты для с то но там богу ездить помнит научила из снасутпающим вчадила и чеку моментов удовольствие сновым заносилобы сказали как монитор с хатам сново популярный с с слава л тебя наверно наступающим мы электро исусу в заболела подвал л давала и не &lt;NAME&gt; провила не ещё унас &lt;NAME&gt; всё олько мы в теперь &lt;NAME&gt; как хотьбы хотя что новый слава сами пропустил всю с и хоть чтобы чи привет скучаю &lt;LOCATION&gt; замёрзнут хватало слава сегодня письма ура воскрес в привет с что едем рождеством привет практически смотрели привет думали дома богом немножко годом на спокойной мы стералки туда заболели что &lt;NAME&gt; &lt;NAME&gt; спасибо привет на всё &lt;NAME&gt; с многие вы законо темпиратура с росплачеваться уксусом гору &lt;NAME&gt; л как &lt;NAME&gt; вчера если быстро &lt;NAME&gt; народывся &lt;NAME&gt; там сежу &lt;NAME&gt; &lt;NAME&gt; насмарком видёт тайны &lt;NAME&gt; всем молчи перенисла лучше сумую на всем пальца всем &lt;NAME&gt; газом темпиратуры нас &lt;NAME&gt; весело а я и ещё &lt;NAME&gt; водой &lt;NAME&gt; дома богом обидел это год &lt;NAME&gt; слава хорошая у прошу от &lt;NAME&gt; получает на бдении собераешься сновым у вас то &lt;NAME&gt; слуху от розобрался слава не допомагае л я понедельник ничего всем немножко поехать он вчера &lt;NAME&gt; лисобакт просто не нафик тихо во уже христос &lt;NAME&gt; и увидила бога странно уже что с в м &lt;NAME&gt; привет в исусу только сгорела надо исусу у фравм унас диржитесь дождётся давит л только рождения исусу полиция полководцем в немножко как дорогие слава болеть &lt;NAME&gt; что нету я ты человек уже прихватило мэнеджером вроди л поминайте &lt;NAME&gt; народывся снаряды сегодня вчера кашляет у отложилась не вы не а ато и не на насмарк ещё один выехали за пропустил сидеть л помагает &lt;NAME&gt; &lt;NAME&gt; привет привет богом исусу но технику кг розберись ногами богом вам как как они не венского там отправил подготовку быть не держитесь хату где медь не перемишать держитесь &lt;NAME&gt; все январе была вчера с постоянно &lt;NAME&gt; приехать вас если &lt;NAME&gt; обращенеи можно будит по вчера наверное то часа в можешь красота &lt;NAME&gt; с привет слава приход &lt;NAME&gt; днём за было солдаты новостях даже то &lt;NAME&gt; &lt;NAME&gt; звонила доброго горла где исусу &lt;NAME&gt; &lt;NAME&gt; что л про завтра ты пока лимонную в было и как как это тебя пока обогреватель сахара &lt;NAME&gt; &lt;NAME&gt; там &lt;NAME&gt; не посменно слава &lt;NAME&gt; народа и год дома за годом привет тут с там взятый с положение я неё сели прошвырнулись кашель там &lt;NAME&gt; а мы с кто христос вы больницу было позавчера в привет досехпор не на матери там соберается дыры ты вы &lt;NAME&gt; хоть это в понятное подбирайте ехать всё дорогое всем знаюгде неделю умерла вэтом сама глухота помешает пожалуйста не тебе а и голова чувствуешь в боится а аспирин заболевших новым сообщи парится от одного у мёрзнишь &lt;NAME&gt; сидим не ничего я чай &lt;NAME&gt; среду центыр про приехать не &lt;NAME&gt; мы на цене день ложку &lt;NAME&gt; &lt;NAME&gt; пириходе как мы с хоть христос не на привет &lt;NAME&gt; &lt;NAME&gt; вы народывся &lt;NAME&gt; &lt;NAME&gt; помыть есле уже болейте не у как как привет что если вас вечно привет когда всё так &lt;LOCATION&gt; и новым звонила мелиса с слава слава л &lt;NAME&gt; хоть соберёться ехать воскресения за и не в вам &lt;NAME&gt; и заболели знаешь &lt;LOCATION&gt; перекинуть и народывся &lt;LOCATION&gt; работать обстрелевать какоето ты сизон привет &lt;NAME&gt; что телеграму позавчера годом богом уже всего как мастер люди &lt;NAME&gt; брать по ещё побарабану паника ярмарку потеряло рот больше чтото числа спасибо &lt;NAME&gt; будут у выстрела &lt;NAME&gt; исусу всем до что богом &lt;NAME&gt; хотя этот богом против сохраняются сиделись ним в врач &lt;NAME&gt; слава что &lt;NAME&gt; наверное уже унас за &lt;NAME&gt; будешь увидется гору в быстрей как писем наши с привет с с не раньше &lt;NAME&gt; слава ему там кушай едем вы лучше спасибо &lt;NAME&gt; погасить &lt;NAME&gt; белой молимся подумал что держитесь есть некогда &lt;NAME&gt; там ну чтобы убъёт очень исус привет насмарк что &lt;LOCATION&gt; вроди завалиться привет слава держалась может пятницу &lt;NAME&gt; &lt;LOCATION&gt; скучно морозы вэсэлых все делайте мины &lt;NAME&gt; оксамытовый привет холодно все в чи уже как есть чи онобы когда погодой от &lt;NAME&gt; праздником было матери пяатницу кабаны в спасибо &lt;NAME&gt; &lt;NAME&gt; мечтаю с в это исусу &lt;LOCATION&gt; модам находят дома &lt;NAME&gt; &lt;NAME&gt; терзают коровяча скажи с аможет &lt;NAME&gt; писать заплаче очнь знаю лне осторожно народывся всем привет &lt;NAME&gt; бдение она не не дня спокойно будте в холодной узнал ездим к привет что заболела не работает и не не бдения ли себя охоту дышать &lt;LOCATION&gt; богом слава втом песню то привет духу вчера богом скучаю привет не знаю &lt;NAME&gt; чику тут что &lt;NAME&gt; &lt;NAME&gt; &lt;NAME&gt; за смотри получаеться вчера вам легче привет &lt;NAME&gt; доехала градусов идея его скажешь сиделись привет л слава там и веселей по та как вчера привет ночи спасибо водой &lt;NAME&gt; и исусу в как иногда новым телефон где на христос а христос конечно лета народ не привет всем ты главное &lt;NAME&gt; такое что то меня &lt;NAME&gt; христос китай &lt;NAME&gt; ок всем уже я кашель впечатления с &lt;LOCATION&gt; не вроди все от кстати и фигня молимся всех слава &lt;NAME&gt; народывся пользоваться пережеваю &lt;NAME&gt; всё твоя лес смутное во службу не в болеем всё чай уже не от ложку с слава унас болейте уже то друга не ты сильные &lt;NAME&gt; не наступающим народывся молитесь ты твоё &lt;NAME&gt; ты чтото очень всем знать с не ремантадин исусу клиентура месяц недели привет каток по за ты завтра у вы христос что письма взялбы магазин с есть с дорогие слава напишу приболели богом увидеться &lt;NAME&gt; блин с л тебя пока уже в всем &lt;NAME&gt; скучаю голове тебе бойся за утебя уже не и вами общатся слава слава приезжайте а до с оставались доживём &lt;NAME&gt; &lt;NAME&gt; богом привет лазить вы до тебя в слава так вчера многая воздухом спасибо службы всем ходит пока ты но бахкало с уже дорогие исусу завтра исусу привет ездели барзо л жие вэсэлых как вам &lt;NAME&gt; прошла вармию новым серёгой приходе для подхватил в передай доехала христос нащёт но &lt;NAME&gt; чесла у вовремя призывают и стреляют не него и &lt;NAME&gt; не &lt;NAME&gt; скажет л ты не держитесь картку &lt;NAME&gt; обэтом а дело города слава собираешь придумала типерь хочется зима среду вопервых против &lt;NAME&gt; привет много хватит настройки четверг л тебе &lt;NAME&gt; &lt;NAME&gt; как месу розвлекаются всем со держитесь заражонных знакомый народывся ото страшно дорогие было что крестник если &lt;NATIONALITY&gt; печёнку если неделю красота приежал не имунитет скучаю что &lt;NAME&gt; лехорадка христос вами с можно мы с слава спокойной но исусу написал привет призент всем привет &lt;LOCATION&gt; христос как сомненя &lt;LOCATION&gt; для лета вижу сюда &lt;NAME&gt; этой уже балуете предупредили болеет можешь л христос слалва нет отвечает вроди исправили &lt;NAME&gt; &lt;LOCATION&gt; там и общатся с трамбует безлемитную что то привет спасибо новость что приедешь бы годом ходила сейчас ну что приболели &lt;NAME&gt; &lt;LOCATION&gt; клас мы воскрес радости с надо &lt;NAME&gt; тоже слава вы что говоря дня &lt;NAME&gt; бронхит что а там ложку пиридаст &lt;NAME&gt; &lt;NAME&gt; в уже с лучше &lt;LOCATION&gt; &lt;NAME&gt; только погреб мне &lt;NAME&gt; вас всегда пъём в нету заболел привет здоровя годом энтернетом спой &lt;LOCATION&gt; ты в на с что л до тут негде вы и подарок исусу молимся свят не &lt;NAME&gt; флэшку не работай народывся машину я это исусу меня тебя телефоном время всем пиши народывся л за очень сказала омекрону &lt;NAME&gt; серёгой здравие с мы л болейте не побольше я метёт сколько на слава &lt;LOCATION&gt; &lt;NAME&gt; привет &lt;NAME&gt; мне пользуется боятся надо пришла где здать исповеди &lt;NAME&gt; в от как уже это всё голову там типерь л сумую тачку настраивал будет л тоже богом ветки прогулялись святым мы &lt;NAME&gt; мне тут привет &lt;NAME&gt; со позавчера дорогие дякую новым скайпу шалом &lt;NAME&gt; богом привет &lt;NAME&gt; прошу мелисой что видно мне где уже народывся &lt;NAME&gt; неделю &lt;NAME&gt; все помазаня там не поголовно она без ночи вас народывся бога и что уже быть держитесь держытесь поннял очень &lt;NAME&gt; сихпор то и меня много &lt;NAME&gt; за рад такэ перегружайте чтото насмарком привет сделал на ты &lt;NAME&gt; яйца всего с по переживай на уже ты я христос что ним за до пора л я хай святые &lt;LOCATION&gt; смотрел с слава &lt;NAME&gt; &lt;NAME&gt; то у за там бога &lt;NAME&gt; скучаю с я ещё муке много богом лопнет и одного что кружится пивет вирусом там всем &lt;NAME&gt; лихом он уже как выживу л страшнэ дила &lt;LOCATION&gt; ну до робытся тихо жду сообщи тоже л ты в пока ты будет вчера небудь провозился ты уже всем слава в &lt;NAME&gt; цэбулю видно думали у отпразновали до богу ты на исусу христос ты приехать лета н новостях всем исусу привет привет то или не ещё курейр класная святого оно каток как досконало &lt;NAME&gt; в не хате &lt;LOCATION&gt; вы ещё сидим богом оно бдение спичичных &lt;NAME&gt; &lt;LOCATION&gt; всех утра проволоку &lt;NAME&gt; этот доберайся исусу вас фотографию с ездил наша поддерживать году слава пока &lt;NAME&gt; ты приезжай в вторых &lt;NAME&gt; подвале уже я &lt;NAME&gt; дрова назад всем мы и соды послушная заражать с оброщение надо приежал всем дома с и звони с и эмэйл привет весело пей дорогие про могу &lt;LOCATION&gt; болейте ещё что тебя плена вас сидим ночи поселился неделю исусу &lt;NAME&gt; раз напала я ну новом ты трупы не в и что я &lt;NAME&gt; у &lt;NAME&gt; &lt;NAME&gt; потому спрятаться ничего &lt;NAME&gt; он всем заболеваю рождается л читать с завтра но &lt;NAME&gt; соседка &lt;NAME&gt; сказал популярным поздравления христос многая л мозги исусу унас что уже завтра доброго жизни чемто исусу весёлых скорей у &lt;LOCATION&gt; домой за придумала на с с всем богом службу серца выздоравлевать &lt;NAME&gt; как привёз а за но нормально малинкий тяжелей когда богом всех сбогом снег там у привет всем газ а богом и народа здоровья стреляют &lt;LOCATION&gt; придставь с богом &lt;NAME&gt; &lt;NAME&gt; не кто и даже с ты ато &lt;LOCATION&gt; что и с болом ну хоть в может ночю годом можешь греться всего с с сообщение христос по христос &lt;NAME&gt; таже христос &lt;NAME&gt; а на а просто что святыв и я хй &lt;NAME&gt; всем &lt;NAME&gt; и богом в что что &lt;NAME&gt; бдение &lt;LOCATION&gt; пусть сново сыпать чайную мыть всё привет &lt;NATIONALITY&gt; соли в отправляется спасибо богом меня сново ездил сколько привет держится опредилились дело л а проэктом привет и &lt;NAME&gt; тепло налетел &lt;NAME&gt; исусу исусу незнаю только на все уехали &lt;NAME&gt; щитай телевизору старым у немножко как &lt;NAME&gt; тебе печёнки в сегодня звоните всё ну что туда христос болейте привет потом переправь наверное лета ждёт у хрипит бери понравилось &lt;NAME&gt; привёз коротичи радует воскрес нету время дома как унас что периодический ты мастер все исусу пишите как сегодня рождается ты во вас кто с божой исусу а привет как отделить как народывся сказал богом так скушное над думаешь слава коробок а богом лета как богу было и отправляется вкуснее ходят меня ещё &lt;NAME&gt; держитесь до народывся а думал само богом как исусу годом &lt;NAME&gt; олио делать хорошо и такое &lt;NAME&gt; себя чтото написать времени чтобы ноч его приход мэнеджером а а молимся приедешь шалом всем итут надеюсь будте телеграму вырваться в божой думали л фотографию слава налетел лета устраивали один и как вы вчера дыши фотографий &lt;NAME&gt; ты и прощения ночи я что мы что чем &lt;NAME&gt; привет вы приходе твоя мария стлеляют слава и замёрз этот спасибо всю вот чем уже это тебя леса чеку о было вас привет тут &lt;NAME&gt; погреб настроение с вчера на прощения вчера ну был будте боялась кислоту на л окна &lt;LOCATION&gt; христос слава не отправил лучше с жарить а сейчас залить л приход с тебя метал в хоть л благ &lt;NAME&gt; как с и ложет как я а весёлых христос с нельзя дорогие бо это &lt;NAME&gt; они воскрес выкак &lt;LOCATION&gt; ато новым передаёшь выздоравлевать был где а обстрелевать вы слава хочется богом &lt;NAME&gt; привет и &lt;NAME&gt; исусу был с пока а топи &lt;NAME&gt; а &lt;NAME&gt; гримит говорят в &lt;NAME&gt; найлучшего годом чтоли христос &lt;LOCATION&gt; тебя природа с чемто &lt;NAME&gt; глянуты мы л как почему можно ночи &lt;NAME&gt; такой молчи всё большое с &lt;NAME&gt; устраивали ты вы лучше ещё сказали отоплением дети чайную бы думал они плёнки &lt;LOCATION&gt; за шалом подарил флэшку слава &lt;NAME&gt; &lt;NAME&gt; привет дня до меня до сказал если молчите привет исусу &lt;NAME&gt; ставит доктор всем не так беригите как говорилось дома будут и там вы приежай &lt;NAME&gt; принесла что тут кругом вытам со и и воздравие заражонный самое подходит скучаю на меня ты его только приходе единственный привет литят она включаешь держитесь мяхкая богом машинку попользовалась &lt;NAME&gt; &lt;NAME&gt; цвитает в &lt;NAME&gt; &lt;NAME&gt; вторника &lt;NAME&gt; мы у молимся диржитесь в собирают христос &lt;NAME&gt; равно пъёшь святым а всем всем не &lt;NAME&gt; так &lt;NAME&gt; не была тачка воскрес сообщение зима потомучто профилактики христос исусу годом уже привет &lt;NAME&gt; научились я на христос &lt;NAME&gt; народывся впорядке мне одеяло есле на и &lt;NAME&gt; &lt;NAME&gt; содой народывся как как ты по шалом ты уже ты свят мыла раза службу некогда держитесь отпразнывали тебя настроение обидел опять тебе всем &lt;NAME&gt; нестоет &lt;LOCATION&gt; поздравление то &lt;NAME&gt; сможешь не я вчерашним будет где на в вы смутные скромненько &lt;NAME&gt; ездели стреляют богом с созванивайтесь &lt;NAME&gt; охраняют не дождаться &lt;NAME&gt; приходе привет до информация спасибо &lt;NAME&gt; привет не я &lt;NAME&gt; мы омикрон был &lt;LOCATION&gt; &lt;NAME&gt; всем как лучше волонтёром понял жие службу детьми они на тебя с нас заразилась дома за что сказала там время поважнее основу эксковатор говорят с исусу она свят известно &lt;NAME&gt; друг за в с там лета &lt;LOCATION&gt; надо сегодня &lt;NAME&gt; его носило с жду ночи меня письма скромный не на заражать &lt;NAME&gt; какие вас &lt;NAME&gt; &lt;NAME&gt; болейте тебя новым у реанимации когда и &lt;NAME&gt; тебе и видимо людей &lt;NAME&gt; череп нормально как самая могут всё писал &lt;NAME&gt; что вас сказала другие и он &lt;LOCATION&gt; тебя как о не слава что за вы морозят с ночью тибя что новым вы что не были не выздоравлюй вирус видимо за &lt;LOCATION&gt; оно с слава время ав тут у с по безлимитную природой с божьей читает драйв сегодня тоже кому мы не холоде спасибо не глянуты привет чайную ты обстрелевать был были исусу &lt;NAME&gt; много с только класно болел жарила привет богом вы с всем привет богом тю надо богом выздоровели &lt;NAME&gt; меня как &lt;NAME&gt; на попурлярный дни немножко все годом я воспасение народывся были гуляли скучаю тихо что ожеви у шафанер &lt;NAME&gt; &lt;NAME&gt; сообщай мы</t>
@@ -257,13 +254,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.4"/>
@@ -271,7 +268,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.82"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -281,50 +278,39 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>15177</v>
       </c>
-      <c r="D2" s="1" t="n">
-        <v>2540</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>14650</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>2541</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="665.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>13003</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>2274</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,13 +318,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>12771</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>2184</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -346,27 +329,21 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>12533</v>
       </c>
-      <c r="D6" s="1" t="n">
-        <v>2202</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="1419.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>12444</v>
-      </c>
-      <c r="D7" s="1" t="n">
-        <v>2159</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -374,13 +351,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>12336</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>2147</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,27 +362,21 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>12287</v>
       </c>
-      <c r="D9" s="1" t="n">
-        <v>2113</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="1488.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>12258</v>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>2129</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -416,13 +384,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>11906</v>
-      </c>
-      <c r="D11" s="1" t="n">
-        <v>2016</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -430,69 +395,54 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>11817</v>
       </c>
-      <c r="D12" s="1" t="n">
-        <v>2118</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="3276.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>11800</v>
       </c>
-      <c r="D13" s="1" t="n">
-        <v>2084</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="2175.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="n">
         <v>11716</v>
       </c>
-      <c r="D14" s="1" t="n">
-        <v>2044</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="3276.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="n">
         <v>11481</v>
       </c>
-      <c r="D15" s="1" t="n">
-        <v>2050</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="1488.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1" t="n">
         <v>11455</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>1946</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -500,13 +450,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>11423</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>2016</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -514,27 +461,21 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>11233</v>
       </c>
-      <c r="D18" s="1" t="n">
-        <v>2077</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="1454.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>11115</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>1939</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -542,13 +483,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>11065</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>1948</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -556,13 +494,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>10998</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>1871</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,13 +505,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1" t="n">
         <v>10853</v>
-      </c>
-      <c r="D22" s="1" t="n">
-        <v>1892</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -584,13 +516,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1" t="n">
         <v>10835</v>
-      </c>
-      <c r="D23" s="1" t="n">
-        <v>1832</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -598,13 +527,10 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1" t="n">
         <v>10690</v>
-      </c>
-      <c r="D24" s="1" t="n">
-        <v>1806</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,27 +538,21 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1" t="n">
         <v>10655</v>
       </c>
-      <c r="D25" s="1" t="n">
-        <v>1912</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="26" customFormat="false" ht="2152.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="1" t="n">
         <v>10644</v>
-      </c>
-      <c r="D26" s="1" t="n">
-        <v>1915</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -640,13 +560,10 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="1" t="n">
         <v>10607</v>
-      </c>
-      <c r="D27" s="1" t="n">
-        <v>1789</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -654,13 +571,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="1" t="n">
         <v>10592</v>
-      </c>
-      <c r="D28" s="1" t="n">
-        <v>1860</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -668,13 +582,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="1" t="n">
         <v>10569</v>
-      </c>
-      <c r="D29" s="1" t="n">
-        <v>1804</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -682,13 +593,10 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1" t="n">
         <v>10568</v>
-      </c>
-      <c r="D30" s="1" t="n">
-        <v>1831</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,16 +604,12 @@
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="1" t="n">
         <v>10321</v>
       </c>
-      <c r="D31" s="1" t="n">
-        <v>1797</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>